<commit_message>
updated data following Rachel's reporting
</commit_message>
<xml_diff>
--- a/analysis/source_data/cleveland/arpa_cle_indirect.xlsx
+++ b/analysis/source_data/cleveland/arpa_cle_indirect.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>County</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Cleveland Police Department</t>
   </si>
   <si>
-    <t>to address homicides and felonious assaults, particularly those committed with firearms, by enhancing the work of its Real-Time Crime Center (RTCC). Operational intelligence and situational awareness will be improved with new technology to help identify wanted suspects.</t>
-  </si>
-  <si>
     <t>retention bonuses for 1,405 sworn officers.</t>
   </si>
   <si>
@@ -93,11 +90,6 @@
   </si>
   <si>
     <t>Cuyahoga County Prosecutor’s Office</t>
-  </si>
-  <si>
-    <t>to create a team of investigators working as part of the Cuyahoga County Crime Gun Intelligence Center who will be assigned exclusively to investigating National Integrated Ballistic Information Network (NIBIN) leads tied to incidents in suburban Cuyahoga County
-communities. These investigators will work with suburban agencies and will assist as
-needed with tasks such as interviewing witnesses and obtaining search warrants.</t>
   </si>
   <si>
     <t>additional attorneys to focus on prosecuting the current backlog of domestic violence and sexual assault cases. Funding will also be used to continue providing forensic phone extractions for law enforcement partners and to conduct a study of the effectiveness of
@@ -107,51 +99,21 @@
     <t>Cuyahoga County Sheriff’s Office</t>
   </si>
   <si>
-    <t>to expand on current efforts to combat violent crime by targeting more resources to hot spot areas with high
-rates of violent crime. The department will increase collaboration with more than 60
-Cuyahoga County law enforcement agencies by offering additional technological
-resources to aid in investigating incidents of violence, preventing crime through general
-deterrence, and increasing the apprehension of violent offenders.</t>
-  </si>
-  <si>
     <t>for retention bonuses for 159 deputies, Ohio Peace Officer Training Academy training, recruitment, advertisements, and to fill 14 vacancies.</t>
   </si>
   <si>
-    <t>East Cleveland</t>
-  </si>
-  <si>
-    <t>East Cleveland Police Department</t>
-  </si>
-  <si>
-    <t>to work to reduce gun violence in their community with new gunshot detection technology to increase response times and improve effectiveness at crime scenes. The
-gunshot detection technology will also allow the department to utilize gunfire location
-and frequency data to identify strategic hot spot locations for future saturation patrols.
-Data will also be used to further develop the community’s comprehensive community
-policing initiative with an emphasis on neighborhoods where community outreach may
-have the highest impact on reducing incidents of gun violence.</t>
+    <t>Euclid, Ohio</t>
+  </si>
+  <si>
+    <t>Euclid Police Department</t>
+  </si>
+  <si>
+    <t>to purchase new technology to assist in preventing and investigating incidents of violent crime.</t>
   </si>
   <si>
     <t>equipment</t>
   </si>
   <si>
-    <t>Euclid, Ohio</t>
-  </si>
-  <si>
-    <t>Euclid Police Department</t>
-  </si>
-  <si>
-    <t>implement a new intelligence-led policing initiative using predictive analysis to target
-gun violence in neighborhood micro-locations. The focused-deterrence initiative will
-create Gun Violence Reduction Teams (GVRT) that will focus solely on these gun
-violence hot spots with the goal of identifying those illegally in possession of firearms,
-increasing gun seizures, and reducing the number of shots fired in these areas. GVRT
-officers will rapidly respond to calls of shots fired to identify and arrest suspects, locate
-and interview witnesses, and provide first aid to any victims.</t>
-  </si>
-  <si>
-    <t>to purchase new technology to assist in preventing and investigating incidents of violent crime.</t>
-  </si>
-  <si>
     <t>City of Garfield Heights</t>
   </si>
   <si>
@@ -204,22 +166,6 @@
   </si>
   <si>
     <t>for hiring three full-time police officers and five full-time dispatchers.</t>
-  </si>
-  <si>
-    <t>City of Westlake</t>
-  </si>
-  <si>
-    <t>Westlake Police Department</t>
-  </si>
-  <si>
-    <t>to work to reduce gun-related crimes and other acts of violence by enhancing its current hot spot  reduce gun-related crimes and other acts of violence by enhancing its current hot spot technology in identified areas with high violent crime rates. Concentrated focus on
-specific hot spots will prevent crime through general deterrence and increased risk of
-apprehension. The Westlake Police Department will also work to engage the community
-through continued problem-oriented policing to address underlying conditions that lead to
-recurring crime problems.</t>
-  </si>
-  <si>
-    <t>equipment&amp;investigations&amp;enforcement</t>
   </si>
   <si>
     <t>Cleveland Heights, Ohio</t>
@@ -620,13 +566,13 @@
         <v>19</v>
       </c>
       <c r="D5" s="3">
-        <v>355400.0</v>
+        <v>4215000.0</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -639,14 +585,14 @@
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3">
-        <v>4215000.0</v>
+      <c r="D6" s="2">
+        <v>1747101.01</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -657,16 +603,16 @@
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2">
-        <v>1747101.01</v>
+        <v>240084.3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -674,19 +620,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2">
-        <v>240084.3</v>
+        <v>989628.3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -694,19 +640,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2">
-        <v>250670.19</v>
+        <v>1532448.48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -714,19 +660,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2">
-        <v>989628.3</v>
+        <v>30</v>
+      </c>
+      <c r="D10" s="3">
+        <v>107000.0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
@@ -734,19 +680,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="3">
-        <v>163000.0</v>
+        <v>34</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1311936.82</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -754,19 +700,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>1532448.48</v>
+        <v>217752.26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -774,19 +720,19 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="2">
-        <v>149236.58</v>
+        <v>40</v>
+      </c>
+      <c r="D13" s="3">
+        <v>216237.0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
@@ -794,16 +740,16 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2">
-        <v>174771.75</v>
+        <v>239689.39</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>10</v>
@@ -814,19 +760,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="3">
-        <v>107000.0</v>
+        <v>46</v>
+      </c>
+      <c r="D15" s="2">
+        <v>382430.34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -834,139 +780,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2">
-        <v>1311936.82</v>
+        <v>1620514.87</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="2">
-        <v>217752.26</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="3">
-        <v>216237.0</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="2">
-        <v>239689.39</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="2">
-        <v>382430.34</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1620514.87</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="3">
-        <v>119250.0</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1012,16 +838,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2">
         <v>72249.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
@@ -1032,13 +858,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3">
         <v>425000.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -1046,16 +872,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D4" s="3">
         <v>400000.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
@@ -1063,16 +889,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3">
         <v>425000.0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -1080,16 +906,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2">
         <v>169093.37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding data review comments and additional analysis
</commit_message>
<xml_diff>
--- a/analysis/source_data/cleveland/arpa_cle_indirect.xlsx
+++ b/analysis/source_data/cleveland/arpa_cle_indirect.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="crime" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="courts" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="from_county" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="courts" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
   <si>
     <t>County</t>
   </si>
@@ -166,6 +167,101 @@
   </si>
   <si>
     <t>for hiring three full-time police officers and five full-time dispatchers.</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Spending Bucket</t>
+  </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>CJ_spending</t>
+  </si>
+  <si>
+    <t>Incentives for Inmates to receive vaccinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuyahoga County </t>
+  </si>
+  <si>
+    <t>direct</t>
+  </si>
+  <si>
+    <t>Public Health</t>
+  </si>
+  <si>
+    <t>courts</t>
+  </si>
+  <si>
+    <t>District 9 - Orange Village for purchasing seven police vehicles - part of $66M allocated equally across each member</t>
+  </si>
+  <si>
+    <t>indirect_county</t>
+  </si>
+  <si>
+    <t>Enhance City Services</t>
+  </si>
+  <si>
+    <t>equiptment</t>
+  </si>
+  <si>
+    <t>District 9 - Village of Woodmere Police Department Body Worn Cameras Replacement Project - part of $66M allocated equally across each member</t>
+  </si>
+  <si>
+    <t>Village of Woodmere</t>
+  </si>
+  <si>
+    <t>Lease of space in Huntington Convention Center and Global Center for Health Innovation for Cuyahoga County Court of Common Pleas jury duty operations</t>
+  </si>
+  <si>
+    <t>Cuyahoga County</t>
+  </si>
+  <si>
+    <t>Enhance County Services</t>
+  </si>
+  <si>
+    <t>Security Camera Network Replacement and Expansion Project from
+the District 10 ARPA Community Grant
+Fund; and declaring the necessity that this
+Resolution become immediately effective</t>
+  </si>
+  <si>
+    <t>City of Cleveland Heights</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> City of Rocky River for the purpose of constructing a
+firearms range for the Rocky River Police
+Department from the District 1 ARPA
+Community Grant Fund; and declaring the
+necessity that this Resolution become
+immediately effective.</t>
+  </si>
+  <si>
+    <t>City of Rocky River</t>
+  </si>
+  <si>
+    <t xml:space="preserve">construction </t>
+  </si>
+  <si>
+    <t>Village of
+Bratenahl for the purpose of purchasing two
+new police vehicles from the District 10
+ARPA Community Grant Fund; and
+declaring the necessity that this Resolution
+become immediately effective</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a total sum, not to exceed
+$50,000, to the City of Maple Heights for the Police Department
+Locker Room Expansion Project from the District 8 ARPA Community
+Grant Fund; and declaring the necessity that this Resolution become
+immediately effective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maple Heights </t>
   </si>
   <si>
     <t>Cleveland Heights, Ohio</t>
@@ -211,11 +307,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -227,22 +324,83 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FFCE9178"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Serif"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E2F3"/>
+        <bgColor rgb="FFD9E2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border/>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -254,6 +412,63 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -268,6 +483,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -474,6 +693,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="18.63"/>
+    <col customWidth="1" min="3" max="3" width="34.75"/>
+    <col customWidth="1" min="5" max="5" width="71.5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -801,6 +1025,239 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9">
+        <v>407500.0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="13">
+        <v>44817.0</v>
+      </c>
+      <c r="G2" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9">
+        <v>274781.57</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="13">
+        <v>44817.0</v>
+      </c>
+      <c r="G3" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9">
+        <v>50006.0</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="13">
+        <v>44817.0</v>
+      </c>
+      <c r="G4" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9">
+        <v>610022.0</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="13">
+        <v>44817.0</v>
+      </c>
+      <c r="G5" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="17">
+        <v>500000.0</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="17">
+        <v>1217000.0</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="21">
+        <v>123235.54</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="22">
+        <v>50000.0</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -838,16 +1295,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2">
         <v>72249.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
@@ -858,13 +1315,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3">
         <v>425000.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
@@ -875,13 +1332,13 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="D4" s="3">
         <v>400000.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
@@ -892,13 +1349,13 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="D5" s="3">
         <v>425000.0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
@@ -906,16 +1363,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="D6" s="2">
         <v>169093.37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>